<commit_message>
Designed a golden reference model with a C++ memory backend
</commit_message>
<xml_diff>
--- a/verification plan/verification plan.xlsx
+++ b/verification plan/verification plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ALL\UNI\courses\Digital circuit\digital github codes\Done\spi\Verification-of-SPI-RAM-UVM\verification plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared Folders\Uni\courses\Digital circuit\digital github codes\Done\spi\Verification-of-SPI-RAM-UVM\verification plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA130E04-55E6-4F0E-817C-FFD3F85D2DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBF371B-8336-4FF9-8B1B-53FB7B78FCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verification Plan" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="140">
   <si>
     <t>#</t>
   </si>
@@ -72,9 +72,6 @@
 reset functionality.</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>Reset Current State</t>
   </si>
   <si>
@@ -291,9 +288,6 @@
   </si>
   <si>
     <t>Signals at IDLE state</t>
-  </si>
-  <si>
-    <t>Verify that the output and internal signals are deasserted at IDLE state (e.g., rx_valid, counter, done_receiving, MISO and rx_data)</t>
   </si>
   <si>
     <t>Assertion: assert_idle</t>
@@ -489,6 +483,9 @@
   </si>
   <si>
     <t>SPI signals checked against golden model.</t>
+  </si>
+  <si>
+    <t>Verify that the output and internal signals are deasserted at IDLE state (e.g., rx_valid and rx_data)</t>
   </si>
 </sst>
 </file>
@@ -1031,25 +1028,25 @@
   </sheetPr>
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="3.21875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="58.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="77.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="50.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="66.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="39.77734375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="3.33203125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="3.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="58.75" style="3" customWidth="1"/>
+    <col min="4" max="4" width="77.625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="50.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="66.125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="39.75" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="3.375" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="31.5" customHeight="1">
@@ -1083,7 +1080,7 @@
       </c>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:13" ht="20.399999999999999">
+    <row r="2" spans="1:13" ht="20.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8">
         <v>1</v>
@@ -1100,7 +1097,7 @@
       <c r="J2" s="21"/>
       <c r="K2" s="13"/>
     </row>
-    <row r="3" spans="1:13" ht="87">
+    <row r="3" spans="1:13" ht="93.75">
       <c r="A3" s="7"/>
       <c r="B3" s="2">
         <v>1.1000000000000001</v>
@@ -1127,26 +1124,26 @@
         <v>100</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="1:13" ht="52.2">
+    <row r="4" spans="1:13" ht="56.25">
       <c r="A4" s="7"/>
       <c r="B4" s="2">
         <v>1.2</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="17" t="s">
         <v>18</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>19</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>14</v>
@@ -1158,7 +1155,7 @@
         <v>100</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K4" s="13"/>
     </row>
@@ -1168,10 +1165,10 @@
         <v>1.3</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>12</v>
@@ -1189,17 +1186,17 @@
         <v>100</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:13" ht="20.399999999999999">
+    <row r="6" spans="1:13" ht="20.25">
       <c r="A6" s="9"/>
       <c r="B6" s="10">
         <v>2</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
@@ -1211,25 +1208,25 @@
       <c r="K6" s="13"/>
       <c r="M6" s="16"/>
     </row>
-    <row r="7" spans="1:13" ht="34.799999999999997">
+    <row r="7" spans="1:13" ht="37.5">
       <c r="A7" s="9"/>
       <c r="B7" s="2">
         <v>2.1</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>25</v>
-      </c>
       <c r="E7" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="2">
         <v>1</v>
@@ -1238,17 +1235,17 @@
         <v>100</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="K7" s="13"/>
     </row>
-    <row r="8" spans="1:13" ht="20.399999999999999">
+    <row r="8" spans="1:13" ht="20.25">
       <c r="A8" s="9"/>
       <c r="B8" s="10">
         <v>3</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
@@ -1259,26 +1256,26 @@
       <c r="J8" s="21"/>
       <c r="K8" s="13"/>
     </row>
-    <row r="9" spans="1:13" ht="52.2">
+    <row r="9" spans="1:13" ht="56.25">
       <c r="A9" s="9"/>
       <c r="B9" s="2">
         <v>3.1</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="E9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="H9" s="2">
         <v>1</v>
       </c>
@@ -1286,30 +1283,30 @@
         <v>100</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K9" s="13"/>
     </row>
-    <row r="10" spans="1:13" ht="52.2">
+    <row r="10" spans="1:13" ht="56.25">
       <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="E10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="H10" s="2">
         <v>1</v>
       </c>
@@ -1317,30 +1314,30 @@
         <v>100</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K10" s="13"/>
     </row>
-    <row r="11" spans="1:13" ht="52.2">
+    <row r="11" spans="1:13" ht="56.25">
       <c r="A11" s="9"/>
       <c r="B11" s="2">
         <v>3.2</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="E11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="H11" s="2">
         <v>1</v>
       </c>
@@ -1348,30 +1345,30 @@
         <v>100</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="1:13" ht="52.2">
+    <row r="12" spans="1:13" ht="56.25">
       <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="E12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="G12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="H12" s="2">
         <v>1</v>
       </c>
@@ -1379,30 +1376,30 @@
         <v>100</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:13" ht="69.599999999999994">
+    <row r="13" spans="1:13" ht="56.25">
       <c r="A13" s="9"/>
       <c r="B13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="E13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="H13" s="2">
         <v>1</v>
       </c>
@@ -1410,30 +1407,30 @@
         <v>100</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="1:13" ht="69.599999999999994">
+    <row r="14" spans="1:13" ht="56.25">
       <c r="A14" s="9"/>
       <c r="B14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="E14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="H14" s="2">
         <v>1</v>
       </c>
@@ -1441,30 +1438,30 @@
         <v>100</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:13" ht="52.2">
+    <row r="15" spans="1:13" ht="56.25">
       <c r="A15" s="7"/>
       <c r="B15" s="2">
         <v>3.3</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="E15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="H15" s="2">
         <v>1</v>
       </c>
@@ -1472,29 +1469,29 @@
         <v>100</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K15" s="13"/>
     </row>
-    <row r="16" spans="1:13" ht="52.2">
+    <row r="16" spans="1:13" ht="56.25">
       <c r="A16" s="7"/>
       <c r="B16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="E16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="F16" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H16" s="2">
         <v>1</v>
@@ -1503,30 +1500,30 @@
         <v>100</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K16" s="13"/>
     </row>
-    <row r="17" spans="1:11" ht="52.2">
+    <row r="17" spans="1:11" ht="56.25">
       <c r="A17" s="7"/>
       <c r="B17" s="2">
         <v>3.4</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="E17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="H17" s="2">
         <v>1</v>
       </c>
@@ -1534,30 +1531,30 @@
         <v>100</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K17" s="13"/>
     </row>
-    <row r="18" spans="1:11" ht="69.599999999999994">
+    <row r="18" spans="1:11" ht="56.25">
       <c r="A18" s="7"/>
       <c r="B18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="E18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="H18" s="2">
         <v>1</v>
       </c>
@@ -1565,30 +1562,30 @@
         <v>100</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K18" s="13"/>
     </row>
-    <row r="19" spans="1:11" ht="52.2">
+    <row r="19" spans="1:11" ht="56.25">
       <c r="A19" s="7"/>
       <c r="B19" s="2">
         <v>3.5</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="E19" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="H19" s="2">
         <v>1</v>
       </c>
@@ -1596,30 +1593,30 @@
         <v>100</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K19" s="13"/>
     </row>
-    <row r="20" spans="1:11" ht="52.2">
+    <row r="20" spans="1:11" ht="56.25">
       <c r="A20" s="7"/>
       <c r="B20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="E20" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F20" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="H20" s="2">
         <v>1</v>
       </c>
@@ -1627,17 +1624,17 @@
         <v>100</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K20" s="13"/>
     </row>
-    <row r="21" spans="1:11" ht="20.399999999999999">
+    <row r="21" spans="1:11" ht="20.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10">
         <v>4</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -1648,26 +1645,26 @@
       <c r="J21" s="21"/>
       <c r="K21" s="13"/>
     </row>
-    <row r="22" spans="1:11" ht="52.2">
+    <row r="22" spans="1:11" ht="56.25">
       <c r="A22" s="7"/>
       <c r="B22" s="2">
         <v>4.0999999999999996</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="H22" s="2">
         <v>1</v>
       </c>
@@ -1675,30 +1672,30 @@
         <v>100</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="K22" s="13"/>
     </row>
-    <row r="23" spans="1:11" ht="52.2">
+    <row r="23" spans="1:11" ht="56.25">
       <c r="A23" s="7"/>
       <c r="B23" s="2">
         <v>4.2</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="F23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="H23" s="2">
         <v>1</v>
       </c>
@@ -1706,17 +1703,17 @@
         <v>100</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="K23" s="13"/>
     </row>
-    <row r="24" spans="1:11" ht="20.399999999999999">
+    <row r="24" spans="1:11" ht="20.25">
       <c r="A24" s="7"/>
       <c r="B24" s="10">
         <v>5</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
@@ -1727,26 +1724,26 @@
       <c r="J24" s="21"/>
       <c r="K24" s="13"/>
     </row>
-    <row r="25" spans="1:11" ht="87">
+    <row r="25" spans="1:11" ht="75">
       <c r="A25" s="7"/>
       <c r="B25" s="2">
         <v>5.0999999999999996</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="F25" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F25" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="H25" s="2">
         <v>1</v>
       </c>
@@ -1754,29 +1751,29 @@
         <v>100</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K25" s="13"/>
     </row>
-    <row r="26" spans="1:11" ht="69.599999999999994">
+    <row r="26" spans="1:11" ht="75">
       <c r="A26" s="7"/>
       <c r="B26" s="2">
         <v>5.2</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="F26" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H26" s="2">
         <v>1</v>
@@ -1785,30 +1782,30 @@
         <v>100</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K26" s="13"/>
     </row>
-    <row r="27" spans="1:11" ht="69.599999999999994">
+    <row r="27" spans="1:11" ht="75">
       <c r="A27" s="7"/>
       <c r="B27" s="2">
         <v>5.3</v>
       </c>
       <c r="C27" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="F27" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F27" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="H27" s="2">
         <v>1</v>
       </c>
@@ -1816,17 +1813,17 @@
         <v>100</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K27" s="13"/>
     </row>
-    <row r="28" spans="1:11" ht="20.399999999999999">
+    <row r="28" spans="1:11" ht="20.25">
       <c r="A28" s="7"/>
       <c r="B28" s="10">
         <v>6</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
@@ -1837,26 +1834,26 @@
       <c r="J28" s="21"/>
       <c r="K28" s="13"/>
     </row>
-    <row r="29" spans="1:11" ht="52.2">
+    <row r="29" spans="1:11" ht="56.25">
       <c r="A29" s="7"/>
       <c r="B29" s="2">
         <v>6.1</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="F29" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F29" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="H29" s="2">
         <v>1</v>
       </c>
@@ -1864,30 +1861,30 @@
         <v>100</v>
       </c>
       <c r="J29" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K29" s="13"/>
     </row>
-    <row r="30" spans="1:11" ht="69.599999999999994">
+    <row r="30" spans="1:11" ht="56.25">
       <c r="A30" s="7"/>
       <c r="B30" s="2">
         <v>6.2</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="F30" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="H30" s="2">
         <v>1</v>
       </c>
@@ -1895,17 +1892,17 @@
         <v>100</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K30" s="13"/>
     </row>
-    <row r="31" spans="1:11" ht="20.399999999999999">
+    <row r="31" spans="1:11" ht="20.25">
       <c r="A31" s="7"/>
       <c r="B31" s="10">
         <v>7</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
@@ -1916,26 +1913,26 @@
       <c r="J31" s="21"/>
       <c r="K31" s="13"/>
     </row>
-    <row r="32" spans="1:11" ht="69.599999999999994">
+    <row r="32" spans="1:11" ht="75">
       <c r="A32" s="7"/>
       <c r="B32" s="2">
         <v>7.1</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="F32" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="H32" s="2">
         <v>1</v>
       </c>
@@ -1943,30 +1940,30 @@
         <v>100</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K32" s="13"/>
     </row>
-    <row r="33" spans="1:11" ht="69.599999999999994">
+    <row r="33" spans="1:11" ht="75">
       <c r="A33" s="7"/>
       <c r="B33" s="2">
         <v>7.2</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="F33" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="H33" s="2">
         <v>1</v>
       </c>
@@ -1974,30 +1971,30 @@
         <v>100</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K33" s="13"/>
     </row>
-    <row r="34" spans="1:11" ht="69.599999999999994">
+    <row r="34" spans="1:11" ht="75">
       <c r="A34" s="7"/>
       <c r="B34" s="2">
         <v>7.3</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="F34" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="H34" s="2">
         <v>1</v>
       </c>
@@ -2005,17 +2002,17 @@
         <v>100</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K34" s="13"/>
     </row>
-    <row r="35" spans="1:11" ht="20.399999999999999">
+    <row r="35" spans="1:11" ht="20.25">
       <c r="A35" s="7"/>
       <c r="B35" s="10">
         <v>8</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
@@ -2026,26 +2023,26 @@
       <c r="J35" s="21"/>
       <c r="K35" s="13"/>
     </row>
-    <row r="36" spans="1:11" ht="87">
+    <row r="36" spans="1:11" ht="93.75">
       <c r="A36" s="7"/>
       <c r="B36" s="2">
         <v>8.1</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="F36" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="H36" s="2">
         <v>1</v>
       </c>
@@ -2053,17 +2050,17 @@
         <v>100</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K36" s="13"/>
     </row>
-    <row r="37" spans="1:11" ht="20.399999999999999">
+    <row r="37" spans="1:11" ht="20.25">
       <c r="A37" s="7"/>
       <c r="B37" s="10">
         <v>9</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="20"/>
@@ -2074,26 +2071,26 @@
       <c r="J37" s="21"/>
       <c r="K37" s="13"/>
     </row>
-    <row r="38" spans="1:11" ht="87">
+    <row r="38" spans="1:11" ht="93.75">
       <c r="A38" s="7"/>
       <c r="B38" s="2">
         <v>9.1</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="E38" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="H38" s="2">
         <v>1</v>
       </c>
@@ -2101,7 +2098,7 @@
         <v>100</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K38" s="13"/>
     </row>

</xml_diff>